<commit_message>
culminacion scrap cuentas b
</commit_message>
<xml_diff>
--- a/2. Proyectos/1. Interpreta Chile/01 Instagram - Proyectos/instagram scraper/url/scrappin_cuentas_b.xlsx
+++ b/2. Proyectos/1. Interpreta Chile/01 Instagram - Proyectos/instagram scraper/url/scrappin_cuentas_b.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10806"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josealonsoordinolaaucca/Documents/Documentos/Vault/Vault/2. Proyectos/1. Interpreta Chile/01 Instagram - Proyectos/instagram scraper/url/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/Proyectos Programacion/Vault - Github/2. Proyectos/1. Interpreta Chile/01 Instagram - Proyectos/instagram scraper/url/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F48DF0E-F070-9B43-AAE7-8FEE26219D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2886B3C-ECD4-A749-B176-7C7A97FCDBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="660" windowWidth="14160" windowHeight="15940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2932,10 +2932,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD75E893-94B7-B44F-8E3F-8CEF6521E78B}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>